<commit_message>
exportar xls reporte operacion unna
se adiciono la opcion de expotar a excel del reporte operacion unna
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/ReporteOSINERGMIN.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/ReporteOSINERGMIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DocEmerson\Github\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F098FF9-F2BD-4821-99DF-A49EEED5FB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900B3FE1-8135-449B-9EFD-00CAA1E47F2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7D5221AC-A4E8-42B5-92F6-57A54FA3EF2A}"/>
+    <workbookView xWindow="20370" yWindow="-3780" windowWidth="20640" windowHeight="11310" xr2:uid="{7D5221AC-A4E8-42B5-92F6-57A54FA3EF2A}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORTE OSINERGMIN" sheetId="1" r:id="rId1"/>
@@ -186,19 +186,10 @@
     <definedName name="VAR">#REF!</definedName>
     <definedName name="VENTAS">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -267,7 +258,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Reporte Operativo del Procesamiento de Gas Natural y Líquidos de Gas Natural</t>
   </si>
@@ -451,12 +442,6 @@
     <t>EVENTOS OPERATIVOS</t>
   </si>
   <si>
-    <t>*Planta de Gas Pariñas:  Planta operando en condiciones normales.</t>
-  </si>
-  <si>
-    <t>{{NombreEmpresa}}</t>
-  </si>
-  <si>
     <t>{{ReporteNro}}</t>
   </si>
   <si>
@@ -464,6 +449,51 @@
   </si>
   <si>
     <t>{{DiaOperativo}}</t>
+  </si>
+  <si>
+    <t>{{EmpresaNombre}}</t>
+  </si>
+  <si>
+    <t>{{CapacidadDisPlanta}}</t>
+  </si>
+  <si>
+    <t>{{VolumenGasNatHumedo}}</t>
+  </si>
+  <si>
+    <t>{{VolumenGasNatSecoReinyFlare}}</t>
+  </si>
+  <si>
+    <t>{{VolumenGasNatSecoVentas}}</t>
+  </si>
+  <si>
+    <t>{{ProcGasNatSecoTotal}}</t>
+  </si>
+  <si>
+    <t>{{olumenLgnProducidoPlanta}}</t>
+  </si>
+  <si>
+    <t>{{VolumenLgnProcesado}}</t>
+  </si>
+  <si>
+    <t>{{VolumenLgnProducidoCgn}}</t>
+  </si>
+  <si>
+    <t>{{VolumenLgnProducidoGlp}}</t>
+  </si>
+  <si>
+    <t>{{VolumenLgnProducidoTotal}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProductosCondensadosLgn}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProductosGlp}}</t>
+  </si>
+  <si>
+    <t>{{VolumenProductosTotal}}</t>
+  </si>
+  <si>
+    <t>{{EventosOperativos}}</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1284,41 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="32" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1284,39 +1347,6 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -30346,7 +30376,7 @@
   <dimension ref="A1:AB84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A38" sqref="A38:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -30367,16 +30397,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="92"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="1"/>
       <c r="L1" s="3" t="s">
         <v>1</v>
@@ -30415,10 +30445,10 @@
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="93" t="s">
-        <v>47</v>
+      <c r="C3" s="85" t="s">
+        <v>45</v>
       </c>
-      <c r="D3" s="94"/>
+      <c r="D3" s="86"/>
       <c r="E3" s="9"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -30466,7 +30496,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
@@ -30519,7 +30549,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="1"/>
@@ -30527,7 +30557,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="1"/>
@@ -30568,16 +30598,16 @@
       </c>
     </row>
     <row r="9" spans="1:28" s="27" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
       <c r="I9" s="1"/>
       <c r="O9" s="4">
         <v>15</v>
@@ -30611,8 +30641,8 @@
       <c r="B11" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="34">
-        <v>44</v>
+      <c r="C11" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>16</v>
@@ -30705,16 +30735,16 @@
       <c r="B15" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="49">
-        <v>25.870999999999999</v>
+      <c r="C15" s="49" t="s">
+        <v>50</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="37"/>
       <c r="F15" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="52">
-        <v>947.61</v>
+      <c r="G15" s="52" t="s">
+        <v>54</v>
       </c>
       <c r="H15" s="38"/>
       <c r="I15" s="1"/>
@@ -30725,10 +30755,10 @@
     </row>
     <row r="16" spans="1:28" s="30" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="44"/>
-      <c r="B16" s="95" t="s">
+      <c r="B16" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="96"/>
+      <c r="C16" s="89"/>
       <c r="D16" s="38"/>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
@@ -30745,8 +30775,8 @@
       <c r="B17" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="54">
-        <v>1.8302499999999995</v>
+      <c r="C17" s="54" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="50"/>
       <c r="E17" s="37"/>
@@ -30770,8 +30800,8 @@
       <c r="B18" s="55" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="56">
-        <v>21.531849999999999</v>
+      <c r="C18" s="56" t="s">
+        <v>52</v>
       </c>
       <c r="D18" s="38"/>
       <c r="E18" s="37"/>
@@ -30795,8 +30825,8 @@
       <c r="B19" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="59">
-        <v>23.362099999999998</v>
+      <c r="C19" s="59" t="s">
+        <v>53</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="37"/>
@@ -30831,16 +30861,16 @@
       <c r="AB20" s="31"/>
     </row>
     <row r="21" spans="1:28" s="30" customFormat="1" ht="31.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="87"/>
+      <c r="E21" s="87"/>
+      <c r="F21" s="87"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="87"/>
       <c r="I21" s="1"/>
       <c r="AB21" s="31"/>
     </row>
@@ -30858,28 +30888,28 @@
     </row>
     <row r="23" spans="1:28" s="30" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="39"/>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="87"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="40"/>
       <c r="E23" s="37"/>
-      <c r="F23" s="86" t="s">
+      <c r="F23" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="87"/>
+      <c r="G23" s="79"/>
       <c r="H23" s="37"/>
       <c r="I23" s="1"/>
       <c r="AB23" s="31"/>
     </row>
     <row r="24" spans="1:28" s="30" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="39"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="81"/>
       <c r="D24" s="40"/>
       <c r="E24" s="37"/>
-      <c r="F24" s="88"/>
-      <c r="G24" s="89"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="81"/>
       <c r="H24" s="37"/>
       <c r="I24" s="1"/>
       <c r="AB24" s="31"/>
@@ -30909,16 +30939,16 @@
       <c r="B26" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="62">
-        <v>947.61</v>
+      <c r="C26" s="62" t="s">
+        <v>55</v>
       </c>
       <c r="D26" s="38"/>
       <c r="E26" s="63"/>
       <c r="F26" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="G26" s="64">
-        <v>261.97000000000003</v>
+      <c r="G26" s="64" t="s">
+        <v>56</v>
       </c>
       <c r="H26" s="38"/>
       <c r="I26" s="1"/>
@@ -30935,8 +30965,8 @@
       <c r="F27" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="67">
-        <v>685.64</v>
+      <c r="G27" s="67" t="s">
+        <v>57</v>
       </c>
       <c r="H27" s="38"/>
       <c r="I27" s="1"/>
@@ -30953,8 +30983,8 @@
       <c r="F28" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="68">
-        <v>947.61</v>
+      <c r="G28" s="68" t="s">
+        <v>58</v>
       </c>
       <c r="H28" s="38"/>
       <c r="I28" s="1"/>
@@ -31025,8 +31055,8 @@
       <c r="F33" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="64">
-        <v>739.11999999999989</v>
+      <c r="G33" s="64" t="s">
+        <v>59</v>
       </c>
       <c r="H33" s="38"/>
       <c r="I33" s="1"/>
@@ -31041,8 +31071,8 @@
       <c r="F34" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="67">
-        <v>4139.49</v>
+      <c r="G34" s="67" t="s">
+        <v>60</v>
       </c>
       <c r="H34" s="38"/>
       <c r="I34" s="1"/>
@@ -31057,8 +31087,8 @@
       <c r="F35" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="G35" s="68">
-        <v>4878.6099999999997</v>
+      <c r="G35" s="68" t="s">
+        <v>61</v>
       </c>
       <c r="H35" s="38"/>
       <c r="I35" s="1"/>
@@ -31077,63 +31107,63 @@
       <c r="AB36" s="31"/>
     </row>
     <row r="37" spans="1:28" s="30" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="78"/>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
-      <c r="E37" s="78"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="78"/>
-      <c r="H37" s="78"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="87"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="87"/>
       <c r="I37" s="1"/>
       <c r="AB37" s="31"/>
     </row>
     <row r="38" spans="1:28" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="79" t="s">
-        <v>45</v>
+      <c r="A38" s="90" t="s">
+        <v>62</v>
       </c>
-      <c r="B38" s="79"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="79"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="79"/>
-      <c r="G38" s="79"/>
-      <c r="H38" s="80"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="90"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="90"/>
+      <c r="H38" s="91"/>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:28" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="81"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
+      <c r="A39" s="92"/>
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
       <c r="I39" s="76"/>
     </row>
     <row r="40" spans="1:28" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="82"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
-      <c r="G40" s="82"/>
-      <c r="H40" s="83"/>
+      <c r="A40" s="93"/>
+      <c r="B40" s="93"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="94"/>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:28" ht="0.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="84"/>
-      <c r="B41" s="84"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="85"/>
+      <c r="A41" s="95"/>
+      <c r="B41" s="95"/>
+      <c r="C41" s="95"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="95"/>
+      <c r="F41" s="95"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="96"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
@@ -31335,6 +31365,11 @@
     <row r="84" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A37:H37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="A39:H39"/>
+    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A41:H41"/>
     <mergeCell ref="B23:C24"/>
     <mergeCell ref="F23:G24"/>
     <mergeCell ref="A1:H1"/>
@@ -31342,11 +31377,6 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="A39:H39"/>
-    <mergeCell ref="A40:H40"/>
-    <mergeCell ref="A41:H41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="47" orientation="portrait" r:id="rId1"/>

</xml_diff>